<commit_message>
Ridership run on 20161026.
</commit_message>
<xml_diff>
--- a/rider/annual/2016.xlsx
+++ b/rider/annual/2016.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="304">
   <si>
     <t>Weekday</t>
   </si>
@@ -833,6 +833,99 @@
   </si>
   <si>
     <t>23 Sep 2016</t>
+  </si>
+  <si>
+    <t>24 Sep 2016</t>
+  </si>
+  <si>
+    <t>25 Sep 2016</t>
+  </si>
+  <si>
+    <t>26 Sep 2016</t>
+  </si>
+  <si>
+    <t>27 Sep 2016</t>
+  </si>
+  <si>
+    <t>28 Sep 2016</t>
+  </si>
+  <si>
+    <t>29 Sep 2016</t>
+  </si>
+  <si>
+    <t>30 Sep 2016</t>
+  </si>
+  <si>
+    <t>01 Oct 2016</t>
+  </si>
+  <si>
+    <t>02 Oct 2016</t>
+  </si>
+  <si>
+    <t>03 Oct 2016</t>
+  </si>
+  <si>
+    <t>04 Oct 2016</t>
+  </si>
+  <si>
+    <t>05 Oct 2016</t>
+  </si>
+  <si>
+    <t>06 Oct 2016</t>
+  </si>
+  <si>
+    <t>07 Oct 2016</t>
+  </si>
+  <si>
+    <t>08 Oct 2016</t>
+  </si>
+  <si>
+    <t>09 Oct 2016</t>
+  </si>
+  <si>
+    <t>11 Oct 2016</t>
+  </si>
+  <si>
+    <t>12 Oct 2016</t>
+  </si>
+  <si>
+    <t>13 Oct 2016</t>
+  </si>
+  <si>
+    <t>14 Oct 2016</t>
+  </si>
+  <si>
+    <t>15 Oct 2016</t>
+  </si>
+  <si>
+    <t>16 Oct 2016</t>
+  </si>
+  <si>
+    <t>17 Oct 2016</t>
+  </si>
+  <si>
+    <t>18 Oct 2016</t>
+  </si>
+  <si>
+    <t>19 Oct 2016</t>
+  </si>
+  <si>
+    <t>20 Oct 2016</t>
+  </si>
+  <si>
+    <t>21 Oct 2016</t>
+  </si>
+  <si>
+    <t>22 Oct 2016</t>
+  </si>
+  <si>
+    <t>23 Oct 2016</t>
+  </si>
+  <si>
+    <t>24 Oct 2016</t>
+  </si>
+  <si>
+    <t>25 Oct 2016</t>
   </si>
 </sst>
 </file>
@@ -923,9 +1016,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Ridership!$B$2:$B$262</c:f>
+              <c:f>Ridership!$B$2:$B$293</c:f>
               <c:strCache>
-                <c:ptCount val="261"/>
+                <c:ptCount val="292"/>
                 <c:pt idx="0">
                   <c:v>02 Jan 2016</c:v>
                 </c:pt>
@@ -1708,16 +1801,109 @@
                 </c:pt>
                 <c:pt idx="260">
                   <c:v>23 Sep 2016</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>24 Sep 2016</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>25 Sep 2016</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>26 Sep 2016</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>27 Sep 2016</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>28 Sep 2016</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>29 Sep 2016</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>30 Sep 2016</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>01 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>02 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>03 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>04 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>05 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>06 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>07 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>08 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>09 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>11 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>12 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>13 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>14 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>15 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>16 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>17 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>18 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>19 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>20 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>21 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>22 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="289">
+                  <c:v>23 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="290">
+                  <c:v>24 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>25 Oct 2016</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Ridership!$C$2:$C$262</c:f>
+              <c:f>Ridership!$C$2:$C$293</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="261"/>
+                <c:ptCount val="292"/>
                 <c:pt idx="0">
                   <c:v>20</c:v>
                 </c:pt>
@@ -2343,19 +2529,19 @@
                   <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="208">
-                  <c:v>185</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="209">
-                  <c:v>181</c:v>
+                  <c:v>171</c:v>
                 </c:pt>
                 <c:pt idx="210">
-                  <c:v>193</c:v>
+                  <c:v>209</c:v>
                 </c:pt>
                 <c:pt idx="211">
-                  <c:v>173</c:v>
+                  <c:v>168</c:v>
                 </c:pt>
                 <c:pt idx="212">
-                  <c:v>179</c:v>
+                  <c:v>184</c:v>
                 </c:pt>
                 <c:pt idx="213">
                   <c:v>69</c:v>
@@ -2364,142 +2550,235 @@
                   <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="215">
-                  <c:v>141</c:v>
+                  <c:v>139</c:v>
                 </c:pt>
                 <c:pt idx="216">
+                  <c:v>219</c:v>
+                </c:pt>
+                <c:pt idx="217">
                   <c:v>213</c:v>
                 </c:pt>
-                <c:pt idx="217">
-                  <c:v>192</c:v>
-                </c:pt>
                 <c:pt idx="218">
-                  <c:v>211</c:v>
+                  <c:v>195</c:v>
                 </c:pt>
                 <c:pt idx="219">
-                  <c:v>253</c:v>
+                  <c:v>249</c:v>
                 </c:pt>
                 <c:pt idx="220">
-                  <c:v>101</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="221">
-                  <c:v>73</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="222">
-                  <c:v>178</c:v>
+                  <c:v>182</c:v>
                 </c:pt>
                 <c:pt idx="223">
-                  <c:v>180</c:v>
+                  <c:v>184</c:v>
                 </c:pt>
                 <c:pt idx="224">
-                  <c:v>199</c:v>
+                  <c:v>177</c:v>
                 </c:pt>
                 <c:pt idx="225">
-                  <c:v>221</c:v>
+                  <c:v>236</c:v>
                 </c:pt>
                 <c:pt idx="226">
-                  <c:v>203</c:v>
+                  <c:v>201</c:v>
                 </c:pt>
                 <c:pt idx="227">
-                  <c:v>84</c:v>
+                  <c:v>87</c:v>
                 </c:pt>
                 <c:pt idx="228">
                   <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="229">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>198</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>206</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>189</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>303</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>229</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>251</c:v>
+                </c:pt>
+                <c:pt idx="238">
                   <c:v>173</c:v>
                 </c:pt>
-                <c:pt idx="230">
-                  <c:v>183</c:v>
-                </c:pt>
-                <c:pt idx="231">
-                  <c:v>180</c:v>
-                </c:pt>
-                <c:pt idx="232">
-                  <c:v>211</c:v>
-                </c:pt>
-                <c:pt idx="233">
-                  <c:v>190</c:v>
-                </c:pt>
-                <c:pt idx="234">
-                  <c:v>294</c:v>
-                </c:pt>
-                <c:pt idx="235">
-                  <c:v>116</c:v>
-                </c:pt>
-                <c:pt idx="236">
-                  <c:v>226</c:v>
-                </c:pt>
-                <c:pt idx="237">
-                  <c:v>233</c:v>
-                </c:pt>
-                <c:pt idx="238">
-                  <c:v>223</c:v>
-                </c:pt>
                 <c:pt idx="239">
-                  <c:v>199</c:v>
+                  <c:v>193</c:v>
                 </c:pt>
                 <c:pt idx="240">
-                  <c:v>137</c:v>
+                  <c:v>149</c:v>
                 </c:pt>
                 <c:pt idx="241">
                   <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="242">
-                  <c:v>80</c:v>
+                  <c:v>77</c:v>
                 </c:pt>
                 <c:pt idx="243">
+                  <c:v>183</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>227</c:v>
+                </c:pt>
+                <c:pt idx="246">
                   <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="244">
-                  <c:v>221</c:v>
-                </c:pt>
-                <c:pt idx="245">
-                  <c:v>222</c:v>
-                </c:pt>
-                <c:pt idx="246">
-                  <c:v>219</c:v>
                 </c:pt>
                 <c:pt idx="247">
                   <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="248">
-                  <c:v>74</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="249">
-                  <c:v>203</c:v>
+                  <c:v>172</c:v>
                 </c:pt>
                 <c:pt idx="250">
-                  <c:v>237</c:v>
+                  <c:v>258</c:v>
                 </c:pt>
                 <c:pt idx="251">
-                  <c:v>209</c:v>
+                  <c:v>240</c:v>
                 </c:pt>
                 <c:pt idx="252">
-                  <c:v>252</c:v>
+                  <c:v>220</c:v>
                 </c:pt>
                 <c:pt idx="253">
-                  <c:v>220</c:v>
+                  <c:v>212</c:v>
                 </c:pt>
                 <c:pt idx="254">
                   <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="255">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>229</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>219</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>222</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>223</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>189</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>178</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>199</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>266</c:v>
+                </c:pt>
+                <c:pt idx="268">
                   <c:v>75</c:v>
                 </c:pt>
-                <c:pt idx="256">
-                  <c:v>217</c:v>
-                </c:pt>
-                <c:pt idx="257">
+                <c:pt idx="269">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>284</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>253</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>297</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>238</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>233</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>253</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>294</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>253</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="289">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="290">
+                  <c:v>252</c:v>
+                </c:pt>
+                <c:pt idx="291">
                   <c:v>239</c:v>
-                </c:pt>
-                <c:pt idx="258">
-                  <c:v>215</c:v>
-                </c:pt>
-                <c:pt idx="259">
-                  <c:v>180</c:v>
-                </c:pt>
-                <c:pt idx="260">
-                  <c:v>277</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2523,9 +2802,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Ridership!$B$2:$B$262</c:f>
+              <c:f>Ridership!$B$2:$B$293</c:f>
               <c:strCache>
-                <c:ptCount val="261"/>
+                <c:ptCount val="292"/>
                 <c:pt idx="0">
                   <c:v>02 Jan 2016</c:v>
                 </c:pt>
@@ -3308,16 +3587,109 @@
                 </c:pt>
                 <c:pt idx="260">
                   <c:v>23 Sep 2016</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>24 Sep 2016</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>25 Sep 2016</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>26 Sep 2016</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>27 Sep 2016</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>28 Sep 2016</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>29 Sep 2016</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>30 Sep 2016</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>01 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>02 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>03 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>04 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>05 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>06 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>07 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>08 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>09 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>11 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>12 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>13 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>14 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>15 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>16 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>17 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>18 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>19 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>20 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>21 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>22 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="289">
+                  <c:v>23 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="290">
+                  <c:v>24 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>25 Oct 2016</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Ridership!$D$2:$D$262</c:f>
+              <c:f>Ridership!$D$2:$D$293</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="261"/>
+                <c:ptCount val="292"/>
                 <c:pt idx="0">
                   <c:v>19.13</c:v>
                 </c:pt>
@@ -3943,19 +4315,19 @@
                   <c:v>32.98</c:v>
                 </c:pt>
                 <c:pt idx="208">
-                  <c:v>92.6</c:v>
+                  <c:v>92.49</c:v>
                 </c:pt>
                 <c:pt idx="209">
-                  <c:v>93.8</c:v>
+                  <c:v>93.59</c:v>
                 </c:pt>
                 <c:pt idx="210">
-                  <c:v>100.02</c:v>
+                  <c:v>100.35</c:v>
                 </c:pt>
                 <c:pt idx="211">
-                  <c:v>97.58</c:v>
+                  <c:v>97.48</c:v>
                 </c:pt>
                 <c:pt idx="212">
-                  <c:v>94.27</c:v>
+                  <c:v>94.38</c:v>
                 </c:pt>
                 <c:pt idx="213">
                   <c:v>40.37</c:v>
@@ -3964,142 +4336,235 @@
                   <c:v>33.17</c:v>
                 </c:pt>
                 <c:pt idx="215">
-                  <c:v>93.7</c:v>
+                  <c:v>93.55</c:v>
                 </c:pt>
                 <c:pt idx="216">
-                  <c:v>96.18</c:v>
+                  <c:v>96.1</c:v>
                 </c:pt>
                 <c:pt idx="217">
-                  <c:v>101.9</c:v>
+                  <c:v>102.65</c:v>
                 </c:pt>
                 <c:pt idx="218">
-                  <c:v>99.9</c:v>
+                  <c:v>99.47</c:v>
                 </c:pt>
                 <c:pt idx="219">
-                  <c:v>97.72</c:v>
+                  <c:v>97.74</c:v>
                 </c:pt>
                 <c:pt idx="220">
-                  <c:v>41.66</c:v>
+                  <c:v>41.64</c:v>
                 </c:pt>
                 <c:pt idx="221">
-                  <c:v>34</c:v>
+                  <c:v>33.98</c:v>
                 </c:pt>
                 <c:pt idx="222">
-                  <c:v>95.58</c:v>
+                  <c:v>95.51</c:v>
                 </c:pt>
                 <c:pt idx="223">
                   <c:v>97.82</c:v>
                 </c:pt>
                 <c:pt idx="224">
-                  <c:v>103.84</c:v>
+                  <c:v>104.14</c:v>
                 </c:pt>
                 <c:pt idx="225">
-                  <c:v>102.32</c:v>
+                  <c:v>102.2</c:v>
                 </c:pt>
                 <c:pt idx="226">
-                  <c:v>99.96</c:v>
+                  <c:v>99.94</c:v>
                 </c:pt>
                 <c:pt idx="227">
-                  <c:v>42.54</c:v>
+                  <c:v>42.58</c:v>
                 </c:pt>
                 <c:pt idx="228">
-                  <c:v>35.02</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="229">
-                  <c:v>97.26</c:v>
+                  <c:v>97.46</c:v>
                 </c:pt>
                 <c:pt idx="230">
-                  <c:v>99.46</c:v>
+                  <c:v>99.75</c:v>
                 </c:pt>
                 <c:pt idx="231">
-                  <c:v>105.33</c:v>
+                  <c:v>105.84</c:v>
                 </c:pt>
                 <c:pt idx="232">
-                  <c:v>104.45</c:v>
+                  <c:v>104.24</c:v>
                 </c:pt>
                 <c:pt idx="233">
-                  <c:v>101.83</c:v>
+                  <c:v>101.79</c:v>
                 </c:pt>
                 <c:pt idx="234">
-                  <c:v>47.67</c:v>
+                  <c:v>47.9</c:v>
                 </c:pt>
                 <c:pt idx="235">
-                  <c:v>36.64</c:v>
+                  <c:v>36.66</c:v>
                 </c:pt>
                 <c:pt idx="236">
-                  <c:v>100</c:v>
+                  <c:v>100.26</c:v>
                 </c:pt>
                 <c:pt idx="237">
-                  <c:v>101.98</c:v>
+                  <c:v>102.6</c:v>
                 </c:pt>
                 <c:pt idx="238">
-                  <c:v>107.6</c:v>
+                  <c:v>107.13</c:v>
                 </c:pt>
                 <c:pt idx="239">
-                  <c:v>106.27</c:v>
+                  <c:v>105.94</c:v>
                 </c:pt>
                 <c:pt idx="240">
-                  <c:v>102.55</c:v>
+                  <c:v>102.76</c:v>
                 </c:pt>
                 <c:pt idx="241">
-                  <c:v>48.66</c:v>
+                  <c:v>48.88</c:v>
                 </c:pt>
                 <c:pt idx="242">
-                  <c:v>37.49</c:v>
+                  <c:v>37.45</c:v>
                 </c:pt>
                 <c:pt idx="243">
-                  <c:v>103.98</c:v>
+                  <c:v>104.09</c:v>
                 </c:pt>
                 <c:pt idx="244">
-                  <c:v>109.74</c:v>
+                  <c:v>109.64</c:v>
                 </c:pt>
                 <c:pt idx="245">
-                  <c:v>108.45</c:v>
+                  <c:v>108.23</c:v>
                 </c:pt>
                 <c:pt idx="246">
-                  <c:v>104.88</c:v>
+                  <c:v>104.9</c:v>
                 </c:pt>
                 <c:pt idx="247">
-                  <c:v>49.37</c:v>
+                  <c:v>49.59</c:v>
                 </c:pt>
                 <c:pt idx="248">
-                  <c:v>38.19</c:v>
+                  <c:v>38.13</c:v>
                 </c:pt>
                 <c:pt idx="249">
-                  <c:v>102.15</c:v>
+                  <c:v>101.75</c:v>
                 </c:pt>
                 <c:pt idx="250">
-                  <c:v>106.4</c:v>
+                  <c:v>106.89</c:v>
                 </c:pt>
                 <c:pt idx="251">
-                  <c:v>111.57</c:v>
+                  <c:v>112.06</c:v>
                 </c:pt>
                 <c:pt idx="252">
-                  <c:v>111.11</c:v>
+                  <c:v>110.3</c:v>
                 </c:pt>
                 <c:pt idx="253">
-                  <c:v>107.14</c:v>
+                  <c:v>107</c:v>
                 </c:pt>
                 <c:pt idx="254">
-                  <c:v>49.58</c:v>
+                  <c:v>49.79</c:v>
                 </c:pt>
                 <c:pt idx="255">
-                  <c:v>38.89</c:v>
+                  <c:v>38.81</c:v>
                 </c:pt>
                 <c:pt idx="256">
-                  <c:v>104.49</c:v>
+                  <c:v>104.35</c:v>
                 </c:pt>
                 <c:pt idx="257">
-                  <c:v>108.77</c:v>
+                  <c:v>108.89</c:v>
                 </c:pt>
                 <c:pt idx="258">
-                  <c:v>113.45</c:v>
+                  <c:v>114.05</c:v>
                 </c:pt>
                 <c:pt idx="259">
-                  <c:v>112.36</c:v>
+                  <c:v>111.76</c:v>
                 </c:pt>
                 <c:pt idx="260">
-                  <c:v>110.4</c:v>
+                  <c:v>109.94</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>50.87</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>39.33</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>106.72</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>110.3</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>115.2</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>113.32</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>112.89</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>51.31</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>39.65</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>109.25</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>113.29</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>117.61</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>115.12</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>116.3</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>52.36</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>40.12</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>115.41</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>119.6</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>117.5</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>118.47</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>52.79</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>40.53</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>111.15</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>117.98</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>122.56</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>119.8</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>120.91</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>54.02</c:v>
+                </c:pt>
+                <c:pt idx="289">
+                  <c:v>41.6</c:v>
+                </c:pt>
+                <c:pt idx="290">
+                  <c:v>113.81</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>119.97</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4123,9 +4588,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Ridership!$B$2:$B$262</c:f>
+              <c:f>Ridership!$B$2:$B$293</c:f>
               <c:strCache>
-                <c:ptCount val="261"/>
+                <c:ptCount val="292"/>
                 <c:pt idx="0">
                   <c:v>02 Jan 2016</c:v>
                 </c:pt>
@@ -4908,16 +5373,109 @@
                 </c:pt>
                 <c:pt idx="260">
                   <c:v>23 Sep 2016</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>24 Sep 2016</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>25 Sep 2016</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>26 Sep 2016</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>27 Sep 2016</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>28 Sep 2016</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>29 Sep 2016</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>30 Sep 2016</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>01 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>02 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>03 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>04 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>05 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>06 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>07 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>08 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>09 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>11 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>12 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>13 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>14 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>15 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>16 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>17 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>18 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>19 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>20 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>21 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>22 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="289">
+                  <c:v>23 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="290">
+                  <c:v>24 Oct 2016</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>25 Oct 2016</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Ridership!$E$2:$E$262</c:f>
+              <c:f>Ridership!$E$2:$E$293</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="261"/>
+                <c:ptCount val="292"/>
                 <c:pt idx="0">
                   <c:v>39.42</c:v>
                 </c:pt>
@@ -5700,6 +6258,99 @@
                 </c:pt>
                 <c:pt idx="260">
                   <c:v>82.2</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>82.36</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>82.53</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>82.69</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>82.85</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>83.01</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>83.17</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>83.33</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>83.49</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>83.66</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>83.82</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>83.98</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>84.14</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>84.3</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>84.46</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>84.62</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>84.79</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>85.11</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>85.27</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>85.43</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>85.59</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>85.76</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>85.92</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>86.08</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>86.24</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>86.4</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>86.56</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>86.72</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>86.89</c:v>
+                </c:pt>
+                <c:pt idx="289">
+                  <c:v>87.05</c:v>
+                </c:pt>
+                <c:pt idx="290">
+                  <c:v>87.21</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>87.37</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5792,13 +6443,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>264</xdr:row>
+      <xdr:row>295</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>278</xdr:row>
+      <xdr:row>309</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6106,7 +6757,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E262"/>
+  <dimension ref="A1:E293"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -9680,10 +10331,10 @@
         <v>220</v>
       </c>
       <c r="C210">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D210">
-        <v>92.6</v>
+        <v>92.49</v>
       </c>
       <c r="E210">
         <v>73.65</v>
@@ -9697,10 +10348,10 @@
         <v>221</v>
       </c>
       <c r="C211">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="D211">
-        <v>93.8</v>
+        <v>93.59</v>
       </c>
       <c r="E211">
         <v>73.81</v>
@@ -9714,10 +10365,10 @@
         <v>222</v>
       </c>
       <c r="C212">
-        <v>193</v>
+        <v>209</v>
       </c>
       <c r="D212">
-        <v>100.02</v>
+        <v>100.35</v>
       </c>
       <c r="E212">
         <v>73.97</v>
@@ -9731,10 +10382,10 @@
         <v>223</v>
       </c>
       <c r="C213">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="D213">
-        <v>97.58</v>
+        <v>97.48</v>
       </c>
       <c r="E213">
         <v>74.13</v>
@@ -9748,10 +10399,10 @@
         <v>224</v>
       </c>
       <c r="C214">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="D214">
-        <v>94.27</v>
+        <v>94.38</v>
       </c>
       <c r="E214">
         <v>74.29</v>
@@ -9799,10 +10450,10 @@
         <v>227</v>
       </c>
       <c r="C217">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D217">
-        <v>93.7</v>
+        <v>93.55</v>
       </c>
       <c r="E217">
         <v>74.78</v>
@@ -9816,10 +10467,10 @@
         <v>228</v>
       </c>
       <c r="C218">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="D218">
-        <v>96.18</v>
+        <v>96.1</v>
       </c>
       <c r="E218">
         <v>74.94</v>
@@ -9833,10 +10484,10 @@
         <v>229</v>
       </c>
       <c r="C219">
-        <v>192</v>
+        <v>213</v>
       </c>
       <c r="D219">
-        <v>101.9</v>
+        <v>102.65</v>
       </c>
       <c r="E219">
         <v>75.1</v>
@@ -9850,10 +10501,10 @@
         <v>230</v>
       </c>
       <c r="C220">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="D220">
-        <v>99.9</v>
+        <v>99.47</v>
       </c>
       <c r="E220">
         <v>75.26</v>
@@ -9867,10 +10518,10 @@
         <v>231</v>
       </c>
       <c r="C221">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="D221">
-        <v>97.72</v>
+        <v>97.74</v>
       </c>
       <c r="E221">
         <v>75.42</v>
@@ -9884,10 +10535,10 @@
         <v>232</v>
       </c>
       <c r="C222">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D222">
-        <v>41.66</v>
+        <v>41.64</v>
       </c>
       <c r="E222">
         <v>75.58</v>
@@ -9901,10 +10552,10 @@
         <v>233</v>
       </c>
       <c r="C223">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D223">
-        <v>34</v>
+        <v>33.98</v>
       </c>
       <c r="E223">
         <v>75.75</v>
@@ -9918,10 +10569,10 @@
         <v>234</v>
       </c>
       <c r="C224">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="D224">
-        <v>95.58</v>
+        <v>95.51</v>
       </c>
       <c r="E224">
         <v>75.91</v>
@@ -9935,7 +10586,7 @@
         <v>235</v>
       </c>
       <c r="C225">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="D225">
         <v>97.82</v>
@@ -9952,10 +10603,10 @@
         <v>236</v>
       </c>
       <c r="C226">
-        <v>199</v>
+        <v>177</v>
       </c>
       <c r="D226">
-        <v>103.84</v>
+        <v>104.14</v>
       </c>
       <c r="E226">
         <v>76.23</v>
@@ -9969,10 +10620,10 @@
         <v>237</v>
       </c>
       <c r="C227">
-        <v>221</v>
+        <v>236</v>
       </c>
       <c r="D227">
-        <v>102.32</v>
+        <v>102.2</v>
       </c>
       <c r="E227">
         <v>76.39</v>
@@ -9986,10 +10637,10 @@
         <v>238</v>
       </c>
       <c r="C228">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D228">
-        <v>99.96</v>
+        <v>99.94</v>
       </c>
       <c r="E228">
         <v>76.55</v>
@@ -10003,10 +10654,10 @@
         <v>239</v>
       </c>
       <c r="C229">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D229">
-        <v>42.54</v>
+        <v>42.58</v>
       </c>
       <c r="E229">
         <v>76.71</v>
@@ -10023,7 +10674,7 @@
         <v>84</v>
       </c>
       <c r="D230">
-        <v>35.02</v>
+        <v>35</v>
       </c>
       <c r="E230">
         <v>76.88</v>
@@ -10037,10 +10688,10 @@
         <v>241</v>
       </c>
       <c r="C231">
-        <v>173</v>
+        <v>185</v>
       </c>
       <c r="D231">
-        <v>97.26</v>
+        <v>97.46</v>
       </c>
       <c r="E231">
         <v>77.04</v>
@@ -10054,10 +10705,10 @@
         <v>242</v>
       </c>
       <c r="C232">
-        <v>183</v>
+        <v>198</v>
       </c>
       <c r="D232">
-        <v>99.46</v>
+        <v>99.75</v>
       </c>
       <c r="E232">
         <v>77.2</v>
@@ -10071,10 +10722,10 @@
         <v>243</v>
       </c>
       <c r="C233">
-        <v>180</v>
+        <v>191</v>
       </c>
       <c r="D233">
-        <v>105.33</v>
+        <v>105.84</v>
       </c>
       <c r="E233">
         <v>77.36</v>
@@ -10088,10 +10739,10 @@
         <v>244</v>
       </c>
       <c r="C234">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D234">
-        <v>104.45</v>
+        <v>104.24</v>
       </c>
       <c r="E234">
         <v>77.52</v>
@@ -10105,10 +10756,10 @@
         <v>245</v>
       </c>
       <c r="C235">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D235">
-        <v>101.83</v>
+        <v>101.79</v>
       </c>
       <c r="E235">
         <v>77.68</v>
@@ -10122,10 +10773,10 @@
         <v>246</v>
       </c>
       <c r="C236">
-        <v>294</v>
+        <v>303</v>
       </c>
       <c r="D236">
-        <v>47.67</v>
+        <v>47.9</v>
       </c>
       <c r="E236">
         <v>77.84</v>
@@ -10139,10 +10790,10 @@
         <v>247</v>
       </c>
       <c r="C237">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D237">
-        <v>36.64</v>
+        <v>36.66</v>
       </c>
       <c r="E237">
         <v>78.01</v>
@@ -10156,10 +10807,10 @@
         <v>248</v>
       </c>
       <c r="C238">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="D238">
-        <v>100</v>
+        <v>100.26</v>
       </c>
       <c r="E238">
         <v>78.17</v>
@@ -10173,10 +10824,10 @@
         <v>249</v>
       </c>
       <c r="C239">
-        <v>233</v>
+        <v>251</v>
       </c>
       <c r="D239">
-        <v>101.98</v>
+        <v>102.6</v>
       </c>
       <c r="E239">
         <v>78.33</v>
@@ -10190,10 +10841,10 @@
         <v>250</v>
       </c>
       <c r="C240">
-        <v>223</v>
+        <v>173</v>
       </c>
       <c r="D240">
-        <v>107.6</v>
+        <v>107.13</v>
       </c>
       <c r="E240">
         <v>78.49</v>
@@ -10207,10 +10858,10 @@
         <v>251</v>
       </c>
       <c r="C241">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="D241">
-        <v>106.27</v>
+        <v>105.94</v>
       </c>
       <c r="E241">
         <v>78.65</v>
@@ -10224,10 +10875,10 @@
         <v>252</v>
       </c>
       <c r="C242">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="D242">
-        <v>102.55</v>
+        <v>102.76</v>
       </c>
       <c r="E242">
         <v>78.81</v>
@@ -10244,7 +10895,7 @@
         <v>97</v>
       </c>
       <c r="D243">
-        <v>48.66</v>
+        <v>48.88</v>
       </c>
       <c r="E243">
         <v>78.97</v>
@@ -10258,10 +10909,10 @@
         <v>254</v>
       </c>
       <c r="C244">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D244">
-        <v>37.49</v>
+        <v>37.45</v>
       </c>
       <c r="E244">
         <v>79.14</v>
@@ -10275,10 +10926,10 @@
         <v>255</v>
       </c>
       <c r="C245">
-        <v>210</v>
+        <v>183</v>
       </c>
       <c r="D245">
-        <v>103.98</v>
+        <v>104.09</v>
       </c>
       <c r="E245">
         <v>79.46</v>
@@ -10292,10 +10943,10 @@
         <v>256</v>
       </c>
       <c r="C246">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="D246">
-        <v>109.74</v>
+        <v>109.64</v>
       </c>
       <c r="E246">
         <v>79.62</v>
@@ -10309,10 +10960,10 @@
         <v>257</v>
       </c>
       <c r="C247">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="D247">
-        <v>108.45</v>
+        <v>108.23</v>
       </c>
       <c r="E247">
         <v>79.78</v>
@@ -10326,10 +10977,10 @@
         <v>258</v>
       </c>
       <c r="C248">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="D248">
-        <v>104.88</v>
+        <v>104.9</v>
       </c>
       <c r="E248">
         <v>79.94</v>
@@ -10346,7 +10997,7 @@
         <v>85</v>
       </c>
       <c r="D249">
-        <v>49.37</v>
+        <v>49.59</v>
       </c>
       <c r="E249">
         <v>80.1</v>
@@ -10360,10 +11011,10 @@
         <v>260</v>
       </c>
       <c r="C250">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D250">
-        <v>38.19</v>
+        <v>38.13</v>
       </c>
       <c r="E250">
         <v>80.27</v>
@@ -10377,10 +11028,10 @@
         <v>261</v>
       </c>
       <c r="C251">
-        <v>203</v>
+        <v>172</v>
       </c>
       <c r="D251">
-        <v>102.15</v>
+        <v>101.75</v>
       </c>
       <c r="E251">
         <v>80.43</v>
@@ -10394,10 +11045,10 @@
         <v>262</v>
       </c>
       <c r="C252">
-        <v>237</v>
+        <v>258</v>
       </c>
       <c r="D252">
-        <v>106.4</v>
+        <v>106.89</v>
       </c>
       <c r="E252">
         <v>80.59</v>
@@ -10411,10 +11062,10 @@
         <v>263</v>
       </c>
       <c r="C253">
-        <v>209</v>
+        <v>240</v>
       </c>
       <c r="D253">
-        <v>111.57</v>
+        <v>112.06</v>
       </c>
       <c r="E253">
         <v>80.75</v>
@@ -10428,10 +11079,10 @@
         <v>264</v>
       </c>
       <c r="C254">
-        <v>252</v>
+        <v>220</v>
       </c>
       <c r="D254">
-        <v>111.11</v>
+        <v>110.3</v>
       </c>
       <c r="E254">
         <v>80.91</v>
@@ -10445,10 +11096,10 @@
         <v>265</v>
       </c>
       <c r="C255">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="D255">
-        <v>107.14</v>
+        <v>107</v>
       </c>
       <c r="E255">
         <v>81.07</v>
@@ -10465,7 +11116,7 @@
         <v>60</v>
       </c>
       <c r="D256">
-        <v>49.58</v>
+        <v>49.79</v>
       </c>
       <c r="E256">
         <v>81.23</v>
@@ -10479,10 +11130,10 @@
         <v>267</v>
       </c>
       <c r="C257">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D257">
-        <v>38.89</v>
+        <v>38.81</v>
       </c>
       <c r="E257">
         <v>81.4</v>
@@ -10496,10 +11147,10 @@
         <v>268</v>
       </c>
       <c r="C258">
-        <v>217</v>
+        <v>229</v>
       </c>
       <c r="D258">
-        <v>104.49</v>
+        <v>104.35</v>
       </c>
       <c r="E258">
         <v>81.56</v>
@@ -10513,10 +11164,10 @@
         <v>269</v>
       </c>
       <c r="C259">
-        <v>239</v>
+        <v>219</v>
       </c>
       <c r="D259">
-        <v>108.77</v>
+        <v>108.89</v>
       </c>
       <c r="E259">
         <v>81.72</v>
@@ -10530,10 +11181,10 @@
         <v>270</v>
       </c>
       <c r="C260">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="D260">
-        <v>113.45</v>
+        <v>114.05</v>
       </c>
       <c r="E260">
         <v>81.88</v>
@@ -10547,10 +11198,10 @@
         <v>271</v>
       </c>
       <c r="C261">
-        <v>180</v>
+        <v>191</v>
       </c>
       <c r="D261">
-        <v>112.36</v>
+        <v>111.76</v>
       </c>
       <c r="E261">
         <v>82.04</v>
@@ -10564,13 +11215,540 @@
         <v>272</v>
       </c>
       <c r="C262">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="D262">
-        <v>110.4</v>
+        <v>109.94</v>
       </c>
       <c r="E262">
         <v>82.2</v>
+      </c>
+    </row>
+    <row r="263" spans="1:5">
+      <c r="A263" t="s">
+        <v>5</v>
+      </c>
+      <c r="B263" t="s">
+        <v>273</v>
+      </c>
+      <c r="C263">
+        <v>107</v>
+      </c>
+      <c r="D263">
+        <v>50.87</v>
+      </c>
+      <c r="E263">
+        <v>82.36</v>
+      </c>
+    </row>
+    <row r="264" spans="1:5">
+      <c r="A264" t="s">
+        <v>7</v>
+      </c>
+      <c r="B264" t="s">
+        <v>274</v>
+      </c>
+      <c r="C264">
+        <v>67</v>
+      </c>
+      <c r="D264">
+        <v>39.33</v>
+      </c>
+      <c r="E264">
+        <v>82.53</v>
+      </c>
+    </row>
+    <row r="265" spans="1:5">
+      <c r="A265" t="s">
+        <v>9</v>
+      </c>
+      <c r="B265" t="s">
+        <v>275</v>
+      </c>
+      <c r="C265">
+        <v>223</v>
+      </c>
+      <c r="D265">
+        <v>106.72</v>
+      </c>
+      <c r="E265">
+        <v>82.69</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5">
+      <c r="A266" t="s">
+        <v>11</v>
+      </c>
+      <c r="B266" t="s">
+        <v>276</v>
+      </c>
+      <c r="C266">
+        <v>189</v>
+      </c>
+      <c r="D266">
+        <v>110.3</v>
+      </c>
+      <c r="E266">
+        <v>82.85</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5">
+      <c r="A267" t="s">
+        <v>13</v>
+      </c>
+      <c r="B267" t="s">
+        <v>277</v>
+      </c>
+      <c r="C267">
+        <v>178</v>
+      </c>
+      <c r="D267">
+        <v>115.2</v>
+      </c>
+      <c r="E267">
+        <v>83.01</v>
+      </c>
+    </row>
+    <row r="268" spans="1:5">
+      <c r="A268" t="s">
+        <v>15</v>
+      </c>
+      <c r="B268" t="s">
+        <v>278</v>
+      </c>
+      <c r="C268">
+        <v>199</v>
+      </c>
+      <c r="D268">
+        <v>113.32</v>
+      </c>
+      <c r="E268">
+        <v>83.17</v>
+      </c>
+    </row>
+    <row r="269" spans="1:5">
+      <c r="A269" t="s">
+        <v>17</v>
+      </c>
+      <c r="B269" t="s">
+        <v>279</v>
+      </c>
+      <c r="C269">
+        <v>266</v>
+      </c>
+      <c r="D269">
+        <v>112.89</v>
+      </c>
+      <c r="E269">
+        <v>83.33</v>
+      </c>
+    </row>
+    <row r="270" spans="1:5">
+      <c r="A270" t="s">
+        <v>5</v>
+      </c>
+      <c r="B270" t="s">
+        <v>280</v>
+      </c>
+      <c r="C270">
+        <v>75</v>
+      </c>
+      <c r="D270">
+        <v>51.31</v>
+      </c>
+      <c r="E270">
+        <v>83.49</v>
+      </c>
+    </row>
+    <row r="271" spans="1:5">
+      <c r="A271" t="s">
+        <v>7</v>
+      </c>
+      <c r="B271" t="s">
+        <v>281</v>
+      </c>
+      <c r="C271">
+        <v>57</v>
+      </c>
+      <c r="D271">
+        <v>39.65</v>
+      </c>
+      <c r="E271">
+        <v>83.66</v>
+      </c>
+    </row>
+    <row r="272" spans="1:5">
+      <c r="A272" t="s">
+        <v>9</v>
+      </c>
+      <c r="B272" t="s">
+        <v>282</v>
+      </c>
+      <c r="C272">
+        <v>236</v>
+      </c>
+      <c r="D272">
+        <v>109.25</v>
+      </c>
+      <c r="E272">
+        <v>83.82</v>
+      </c>
+    </row>
+    <row r="273" spans="1:5">
+      <c r="A273" t="s">
+        <v>11</v>
+      </c>
+      <c r="B273" t="s">
+        <v>283</v>
+      </c>
+      <c r="C273">
+        <v>284</v>
+      </c>
+      <c r="D273">
+        <v>113.29</v>
+      </c>
+      <c r="E273">
+        <v>83.98</v>
+      </c>
+    </row>
+    <row r="274" spans="1:5">
+      <c r="A274" t="s">
+        <v>13</v>
+      </c>
+      <c r="B274" t="s">
+        <v>284</v>
+      </c>
+      <c r="C274">
+        <v>253</v>
+      </c>
+      <c r="D274">
+        <v>117.61</v>
+      </c>
+      <c r="E274">
+        <v>84.14</v>
+      </c>
+    </row>
+    <row r="275" spans="1:5">
+      <c r="A275" t="s">
+        <v>15</v>
+      </c>
+      <c r="B275" t="s">
+        <v>285</v>
+      </c>
+      <c r="C275">
+        <v>216</v>
+      </c>
+      <c r="D275">
+        <v>115.12</v>
+      </c>
+      <c r="E275">
+        <v>84.3</v>
+      </c>
+    </row>
+    <row r="276" spans="1:5">
+      <c r="A276" t="s">
+        <v>17</v>
+      </c>
+      <c r="B276" t="s">
+        <v>286</v>
+      </c>
+      <c r="C276">
+        <v>297</v>
+      </c>
+      <c r="D276">
+        <v>116.3</v>
+      </c>
+      <c r="E276">
+        <v>84.46</v>
+      </c>
+    </row>
+    <row r="277" spans="1:5">
+      <c r="A277" t="s">
+        <v>5</v>
+      </c>
+      <c r="B277" t="s">
+        <v>287</v>
+      </c>
+      <c r="C277">
+        <v>109</v>
+      </c>
+      <c r="D277">
+        <v>52.36</v>
+      </c>
+      <c r="E277">
+        <v>84.62</v>
+      </c>
+    </row>
+    <row r="278" spans="1:5">
+      <c r="A278" t="s">
+        <v>7</v>
+      </c>
+      <c r="B278" t="s">
+        <v>288</v>
+      </c>
+      <c r="C278">
+        <v>66</v>
+      </c>
+      <c r="D278">
+        <v>40.12</v>
+      </c>
+      <c r="E278">
+        <v>84.79</v>
+      </c>
+    </row>
+    <row r="279" spans="1:5">
+      <c r="A279" t="s">
+        <v>11</v>
+      </c>
+      <c r="B279" t="s">
+        <v>289</v>
+      </c>
+      <c r="C279">
+        <v>238</v>
+      </c>
+      <c r="D279">
+        <v>115.41</v>
+      </c>
+      <c r="E279">
+        <v>85.11</v>
+      </c>
+    </row>
+    <row r="280" spans="1:5">
+      <c r="A280" t="s">
+        <v>13</v>
+      </c>
+      <c r="B280" t="s">
+        <v>290</v>
+      </c>
+      <c r="C280">
+        <v>233</v>
+      </c>
+      <c r="D280">
+        <v>119.6</v>
+      </c>
+      <c r="E280">
+        <v>85.27</v>
+      </c>
+    </row>
+    <row r="281" spans="1:5">
+      <c r="A281" t="s">
+        <v>15</v>
+      </c>
+      <c r="B281" t="s">
+        <v>291</v>
+      </c>
+      <c r="C281">
+        <v>253</v>
+      </c>
+      <c r="D281">
+        <v>117.5</v>
+      </c>
+      <c r="E281">
+        <v>85.43</v>
+      </c>
+    </row>
+    <row r="282" spans="1:5">
+      <c r="A282" t="s">
+        <v>17</v>
+      </c>
+      <c r="B282" t="s">
+        <v>292</v>
+      </c>
+      <c r="C282">
+        <v>236</v>
+      </c>
+      <c r="D282">
+        <v>118.47</v>
+      </c>
+      <c r="E282">
+        <v>85.59</v>
+      </c>
+    </row>
+    <row r="283" spans="1:5">
+      <c r="A283" t="s">
+        <v>5</v>
+      </c>
+      <c r="B283" t="s">
+        <v>293</v>
+      </c>
+      <c r="C283">
+        <v>76</v>
+      </c>
+      <c r="D283">
+        <v>52.79</v>
+      </c>
+      <c r="E283">
+        <v>85.76</v>
+      </c>
+    </row>
+    <row r="284" spans="1:5">
+      <c r="A284" t="s">
+        <v>7</v>
+      </c>
+      <c r="B284" t="s">
+        <v>294</v>
+      </c>
+      <c r="C284">
+        <v>63</v>
+      </c>
+      <c r="D284">
+        <v>40.53</v>
+      </c>
+      <c r="E284">
+        <v>85.92</v>
+      </c>
+    </row>
+    <row r="285" spans="1:5">
+      <c r="A285" t="s">
+        <v>9</v>
+      </c>
+      <c r="B285" t="s">
+        <v>295</v>
+      </c>
+      <c r="C285">
+        <v>208</v>
+      </c>
+      <c r="D285">
+        <v>111.15</v>
+      </c>
+      <c r="E285">
+        <v>86.08</v>
+      </c>
+    </row>
+    <row r="286" spans="1:5">
+      <c r="A286" t="s">
+        <v>11</v>
+      </c>
+      <c r="B286" t="s">
+        <v>296</v>
+      </c>
+      <c r="C286">
+        <v>270</v>
+      </c>
+      <c r="D286">
+        <v>117.98</v>
+      </c>
+      <c r="E286">
+        <v>86.24</v>
+      </c>
+    </row>
+    <row r="287" spans="1:5">
+      <c r="A287" t="s">
+        <v>13</v>
+      </c>
+      <c r="B287" t="s">
+        <v>297</v>
+      </c>
+      <c r="C287">
+        <v>294</v>
+      </c>
+      <c r="D287">
+        <v>122.56</v>
+      </c>
+      <c r="E287">
+        <v>86.4</v>
+      </c>
+    </row>
+    <row r="288" spans="1:5">
+      <c r="A288" t="s">
+        <v>15</v>
+      </c>
+      <c r="B288" t="s">
+        <v>298</v>
+      </c>
+      <c r="C288">
+        <v>253</v>
+      </c>
+      <c r="D288">
+        <v>119.8</v>
+      </c>
+      <c r="E288">
+        <v>86.56</v>
+      </c>
+    </row>
+    <row r="289" spans="1:5">
+      <c r="A289" t="s">
+        <v>17</v>
+      </c>
+      <c r="B289" t="s">
+        <v>299</v>
+      </c>
+      <c r="C289">
+        <v>255</v>
+      </c>
+      <c r="D289">
+        <v>120.91</v>
+      </c>
+      <c r="E289">
+        <v>86.72</v>
+      </c>
+    </row>
+    <row r="290" spans="1:5">
+      <c r="A290" t="s">
+        <v>5</v>
+      </c>
+      <c r="B290" t="s">
+        <v>300</v>
+      </c>
+      <c r="C290">
+        <v>123</v>
+      </c>
+      <c r="D290">
+        <v>54.02</v>
+      </c>
+      <c r="E290">
+        <v>86.89</v>
+      </c>
+    </row>
+    <row r="291" spans="1:5">
+      <c r="A291" t="s">
+        <v>7</v>
+      </c>
+      <c r="B291" t="s">
+        <v>301</v>
+      </c>
+      <c r="C291">
+        <v>103</v>
+      </c>
+      <c r="D291">
+        <v>41.6</v>
+      </c>
+      <c r="E291">
+        <v>87.05</v>
+      </c>
+    </row>
+    <row r="292" spans="1:5">
+      <c r="A292" t="s">
+        <v>9</v>
+      </c>
+      <c r="B292" t="s">
+        <v>302</v>
+      </c>
+      <c r="C292">
+        <v>252</v>
+      </c>
+      <c r="D292">
+        <v>113.81</v>
+      </c>
+      <c r="E292">
+        <v>87.21</v>
+      </c>
+    </row>
+    <row r="293" spans="1:5">
+      <c r="A293" t="s">
+        <v>11</v>
+      </c>
+      <c r="B293" t="s">
+        <v>303</v>
+      </c>
+      <c r="C293">
+        <v>239</v>
+      </c>
+      <c r="D293">
+        <v>119.97</v>
+      </c>
+      <c r="E293">
+        <v>87.37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new Madigan bike hours
</commit_message>
<xml_diff>
--- a/rider/annual/2016.xlsx
+++ b/rider/annual/2016.xlsx
@@ -525,190 +525,190 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="62"/>
                 <c:pt idx="0">
-                  <c:v>279</c:v>
+                  <c:v>281</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>129</c:v>
+                  <c:v>127</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>296</c:v>
+                  <c:v>269</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>254</c:v>
+                  <c:v>260</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>240</c:v>
+                  <c:v>270</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>266</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>234</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>257</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>209</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>232</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>221</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>306</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>212</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>264</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>218</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>94</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>240</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>183</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>230</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>226</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>118</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>73</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>289</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>237</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>290</c:v>
-                </c:pt>
                 <c:pt idx="19">
-                  <c:v>254</c:v>
+                  <c:v>261</c:v>
                 </c:pt>
                 <c:pt idx="20">
+                  <c:v>246</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="23">
                   <c:v>233</c:v>
                 </c:pt>
-                <c:pt idx="21">
-                  <c:v>123</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>103</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>241</c:v>
-                </c:pt>
                 <c:pt idx="24">
-                  <c:v>206</c:v>
+                  <c:v>209</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>213</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>171</c:v>
+                  <c:v>172</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>126</c:v>
+                  <c:v>131</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>98</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>261</c:v>
+                  <c:v>246</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>279</c:v>
+                  <c:v>277</c:v>
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>256</c:v>
+                  <c:v>247</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>263</c:v>
+                  <c:v>253</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>153</c:v>
+                  <c:v>141</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>128</c:v>
+                  <c:v>133</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>224</c:v>
+                  <c:v>273</c:v>
                 </c:pt>
                 <c:pt idx="37">
+                  <c:v>218</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>204</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>141</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>289</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>217</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>241</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>332</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>181</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>284</c:v>
+                </c:pt>
+                <c:pt idx="51">
                   <c:v>227</c:v>
                 </c:pt>
-                <c:pt idx="38">
-                  <c:v>248</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>136</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>81</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>143</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>159</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>282</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>182</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>212</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>274</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>299</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>173</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>147</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>268</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>257</c:v>
-                </c:pt>
                 <c:pt idx="52">
-                  <c:v>204</c:v>
+                  <c:v>202</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>210</c:v>
+                  <c:v>201</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>95</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>44</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>46</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="57">
                   <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>147</c:v>
+                  <c:v>144</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>148</c:v>
+                  <c:v>139</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>354</c:v>
+                  <c:v>357</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>56</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -931,190 +931,190 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="62"/>
                 <c:pt idx="0">
-                  <c:v>279</c:v>
+                  <c:v>281</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>129</c:v>
+                  <c:v>127</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>296</c:v>
+                  <c:v>269</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>254</c:v>
+                  <c:v>260</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>240</c:v>
+                  <c:v>270</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>264</c:v>
+                  <c:v>266</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>248.5</c:v>
+                  <c:v>257.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>111.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>263</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>234.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>251</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>243.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>277.33</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>227</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>255.33</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>249.33</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>253.67</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>116.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>77</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>268</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>218.5</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>235</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>245</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>113.67</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>75.67</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>275</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>224.67</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>253.33</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>248</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>243.33</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>116</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>82.5</c:v>
-                </c:pt>
                 <c:pt idx="23">
-                  <c:v>266.5</c:v>
+                  <c:v>266.25</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>220</c:v>
+                  <c:v>222.5</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>243.25</c:v>
+                  <c:v>241.5</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>225.25</c:v>
+                  <c:v>233.25</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>118</c:v>
+                  <c:v>119.4</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>85.59999999999999</c:v>
+                  <c:v>80.8</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>265.4</c:v>
+                  <c:v>262.2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>231.8</c:v>
+                  <c:v>233.4</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>198.6</c:v>
+                  <c:v>197.2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>250</c:v>
+                  <c:v>248.75</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>232.8</c:v>
+                  <c:v>237.2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>123.83</c:v>
+                  <c:v>123</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>92.67</c:v>
+                  <c:v>89.5</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>258.5</c:v>
+                  <c:v>264</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>231</c:v>
+                  <c:v>230.83</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>206.83</c:v>
+                  <c:v>198.33</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>227.2</c:v>
+                  <c:v>226.4</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>207.5</c:v>
+                  <c:v>211</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>126.57</c:v>
+                  <c:v>125.57</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>102.14</c:v>
+                  <c:v>99.86</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>261.86</c:v>
+                  <c:v>267.57</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>224</c:v>
+                  <c:v>228.86</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>207.57</c:v>
+                  <c:v>197.14</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>235</c:v>
+                  <c:v>228.83</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>220.57</c:v>
+                  <c:v>228.29</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>132.38</c:v>
+                  <c:v>132.5</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>107.75</c:v>
+                  <c:v>105.5</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>262.62</c:v>
+                  <c:v>269.62</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>228.12</c:v>
+                  <c:v>228.62</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>207.12</c:v>
+                  <c:v>197.75</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>231.43</c:v>
+                  <c:v>224.86</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>204.88</c:v>
+                  <c:v>211.25</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>122.56</c:v>
+                  <c:v>122.44</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>238.56</c:v>
+                  <c:v>244.67</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>213.78</c:v>
+                  <c:v>214.22</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>200.44</c:v>
+                  <c:v>191.78</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>221</c:v>
+                  <c:v>214.12</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>221.44</c:v>
+                  <c:v>227.44</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>115.9</c:v>
+                  <c:v>116.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1965,10 +1965,10 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="D2">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="E2">
         <v>87.84999999999999</v>
@@ -1982,10 +1982,10 @@
         <v>8</v>
       </c>
       <c r="C3">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D3">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E3">
         <v>88.02</v>
@@ -2016,10 +2016,10 @@
         <v>12</v>
       </c>
       <c r="C5">
-        <v>296</v>
+        <v>269</v>
       </c>
       <c r="D5">
-        <v>296</v>
+        <v>269</v>
       </c>
       <c r="E5">
         <v>88.34</v>
@@ -2033,10 +2033,10 @@
         <v>14</v>
       </c>
       <c r="C6">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="D6">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="E6">
         <v>88.5</v>
@@ -2050,10 +2050,10 @@
         <v>16</v>
       </c>
       <c r="C7">
-        <v>240</v>
+        <v>270</v>
       </c>
       <c r="D7">
-        <v>240</v>
+        <v>270</v>
       </c>
       <c r="E7">
         <v>88.66</v>
@@ -2067,10 +2067,10 @@
         <v>18</v>
       </c>
       <c r="C8">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="D8">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="E8">
         <v>88.81999999999999</v>
@@ -2084,10 +2084,10 @@
         <v>19</v>
       </c>
       <c r="C9">
-        <v>218</v>
+        <v>234</v>
       </c>
       <c r="D9">
-        <v>248.5</v>
+        <v>257.5</v>
       </c>
       <c r="E9">
         <v>88.98</v>
@@ -2101,7 +2101,7 @@
         <v>20</v>
       </c>
       <c r="C10">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D10">
         <v>111.5</v>
@@ -2118,10 +2118,10 @@
         <v>21</v>
       </c>
       <c r="C11">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D11">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E11">
         <v>89.31</v>
@@ -2135,10 +2135,10 @@
         <v>22</v>
       </c>
       <c r="C12">
-        <v>240</v>
+        <v>257</v>
       </c>
       <c r="D12">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="E12">
         <v>89.47</v>
@@ -2152,10 +2152,10 @@
         <v>23</v>
       </c>
       <c r="C13">
-        <v>183</v>
+        <v>209</v>
       </c>
       <c r="D13">
-        <v>218.5</v>
+        <v>234.5</v>
       </c>
       <c r="E13">
         <v>89.63</v>
@@ -2169,10 +2169,10 @@
         <v>24</v>
       </c>
       <c r="C14">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="D14">
-        <v>235</v>
+        <v>251</v>
       </c>
       <c r="E14">
         <v>89.79000000000001</v>
@@ -2186,10 +2186,10 @@
         <v>25</v>
       </c>
       <c r="C15">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="D15">
-        <v>245</v>
+        <v>243.5</v>
       </c>
       <c r="E15">
         <v>89.95</v>
@@ -2203,10 +2203,10 @@
         <v>26</v>
       </c>
       <c r="C16">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D16">
-        <v>113.67</v>
+        <v>113</v>
       </c>
       <c r="E16">
         <v>90.28</v>
@@ -2220,10 +2220,10 @@
         <v>27</v>
       </c>
       <c r="C17">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D17">
-        <v>75.67</v>
+        <v>74</v>
       </c>
       <c r="E17">
         <v>90.44</v>
@@ -2237,10 +2237,10 @@
         <v>28</v>
       </c>
       <c r="C18">
-        <v>289</v>
+        <v>306</v>
       </c>
       <c r="D18">
-        <v>275</v>
+        <v>277.33</v>
       </c>
       <c r="E18">
         <v>90.59999999999999</v>
@@ -2254,10 +2254,10 @@
         <v>29</v>
       </c>
       <c r="C19">
-        <v>237</v>
+        <v>212</v>
       </c>
       <c r="D19">
-        <v>224.67</v>
+        <v>227</v>
       </c>
       <c r="E19">
         <v>90.76000000000001</v>
@@ -2271,10 +2271,10 @@
         <v>30</v>
       </c>
       <c r="C20">
-        <v>290</v>
+        <v>264</v>
       </c>
       <c r="D20">
-        <v>253.33</v>
+        <v>255.33</v>
       </c>
       <c r="E20">
         <v>90.92</v>
@@ -2288,10 +2288,10 @@
         <v>31</v>
       </c>
       <c r="C21">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="D21">
-        <v>248</v>
+        <v>249.33</v>
       </c>
       <c r="E21">
         <v>91.08</v>
@@ -2305,10 +2305,10 @@
         <v>32</v>
       </c>
       <c r="C22">
-        <v>233</v>
+        <v>246</v>
       </c>
       <c r="D22">
-        <v>243.33</v>
+        <v>253.67</v>
       </c>
       <c r="E22">
         <v>91.23999999999999</v>
@@ -2322,10 +2322,10 @@
         <v>33</v>
       </c>
       <c r="C23">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="D23">
-        <v>116</v>
+        <v>116.5</v>
       </c>
       <c r="E23">
         <v>91.41</v>
@@ -2339,10 +2339,10 @@
         <v>34</v>
       </c>
       <c r="C24">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="D24">
-        <v>82.5</v>
+        <v>77</v>
       </c>
       <c r="E24">
         <v>91.56999999999999</v>
@@ -2356,10 +2356,10 @@
         <v>35</v>
       </c>
       <c r="C25">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="D25">
-        <v>266.5</v>
+        <v>266.25</v>
       </c>
       <c r="E25">
         <v>91.73</v>
@@ -2373,10 +2373,10 @@
         <v>36</v>
       </c>
       <c r="C26">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D26">
-        <v>220</v>
+        <v>222.5</v>
       </c>
       <c r="E26">
         <v>91.89</v>
@@ -2390,10 +2390,10 @@
         <v>37</v>
       </c>
       <c r="C27">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="D27">
-        <v>243.25</v>
+        <v>241.5</v>
       </c>
       <c r="E27">
         <v>92.05</v>
@@ -2407,10 +2407,10 @@
         <v>38</v>
       </c>
       <c r="C28">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D28">
-        <v>225.25</v>
+        <v>233.25</v>
       </c>
       <c r="E28">
         <v>92.37</v>
@@ -2424,10 +2424,10 @@
         <v>39</v>
       </c>
       <c r="C29">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="D29">
-        <v>118</v>
+        <v>119.4</v>
       </c>
       <c r="E29">
         <v>92.54000000000001</v>
@@ -2441,10 +2441,10 @@
         <v>40</v>
       </c>
       <c r="C30">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D30">
-        <v>85.59999999999999</v>
+        <v>80.8</v>
       </c>
       <c r="E30">
         <v>92.7</v>
@@ -2458,10 +2458,10 @@
         <v>41</v>
       </c>
       <c r="C31">
-        <v>261</v>
+        <v>246</v>
       </c>
       <c r="D31">
-        <v>265.4</v>
+        <v>262.2</v>
       </c>
       <c r="E31">
         <v>92.86</v>
@@ -2475,10 +2475,10 @@
         <v>42</v>
       </c>
       <c r="C32">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D32">
-        <v>231.8</v>
+        <v>233.4</v>
       </c>
       <c r="E32">
         <v>93.02</v>
@@ -2495,7 +2495,7 @@
         <v>20</v>
       </c>
       <c r="D33">
-        <v>198.6</v>
+        <v>197.2</v>
       </c>
       <c r="E33">
         <v>93.18000000000001</v>
@@ -2509,10 +2509,10 @@
         <v>44</v>
       </c>
       <c r="C34">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="D34">
-        <v>250</v>
+        <v>248.75</v>
       </c>
       <c r="E34">
         <v>93.34</v>
@@ -2526,10 +2526,10 @@
         <v>45</v>
       </c>
       <c r="C35">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="D35">
-        <v>232.8</v>
+        <v>237.2</v>
       </c>
       <c r="E35">
         <v>93.5</v>
@@ -2543,10 +2543,10 @@
         <v>46</v>
       </c>
       <c r="C36">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="D36">
-        <v>123.83</v>
+        <v>123</v>
       </c>
       <c r="E36">
         <v>93.67</v>
@@ -2560,10 +2560,10 @@
         <v>47</v>
       </c>
       <c r="C37">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="D37">
-        <v>92.67</v>
+        <v>89.5</v>
       </c>
       <c r="E37">
         <v>93.83</v>
@@ -2577,10 +2577,10 @@
         <v>48</v>
       </c>
       <c r="C38">
-        <v>224</v>
+        <v>273</v>
       </c>
       <c r="D38">
-        <v>258.5</v>
+        <v>264</v>
       </c>
       <c r="E38">
         <v>93.98999999999999</v>
@@ -2594,10 +2594,10 @@
         <v>49</v>
       </c>
       <c r="C39">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="D39">
-        <v>231</v>
+        <v>230.83</v>
       </c>
       <c r="E39">
         <v>94.15000000000001</v>
@@ -2611,10 +2611,10 @@
         <v>50</v>
       </c>
       <c r="C40">
-        <v>248</v>
+        <v>204</v>
       </c>
       <c r="D40">
-        <v>206.83</v>
+        <v>198.33</v>
       </c>
       <c r="E40">
         <v>94.31</v>
@@ -2628,10 +2628,10 @@
         <v>51</v>
       </c>
       <c r="C41">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D41">
-        <v>227.2</v>
+        <v>226.4</v>
       </c>
       <c r="E41">
         <v>94.47</v>
@@ -2645,10 +2645,10 @@
         <v>52</v>
       </c>
       <c r="C42">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D42">
-        <v>207.5</v>
+        <v>211</v>
       </c>
       <c r="E42">
         <v>94.63</v>
@@ -2662,10 +2662,10 @@
         <v>53</v>
       </c>
       <c r="C43">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D43">
-        <v>126.57</v>
+        <v>125.57</v>
       </c>
       <c r="E43">
         <v>94.8</v>
@@ -2679,10 +2679,10 @@
         <v>54</v>
       </c>
       <c r="C44">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="D44">
-        <v>102.14</v>
+        <v>99.86</v>
       </c>
       <c r="E44">
         <v>94.95999999999999</v>
@@ -2696,10 +2696,10 @@
         <v>55</v>
       </c>
       <c r="C45">
-        <v>282</v>
+        <v>289</v>
       </c>
       <c r="D45">
-        <v>261.86</v>
+        <v>267.57</v>
       </c>
       <c r="E45">
         <v>95.12</v>
@@ -2713,10 +2713,10 @@
         <v>56</v>
       </c>
       <c r="C46">
-        <v>182</v>
+        <v>217</v>
       </c>
       <c r="D46">
-        <v>224</v>
+        <v>228.86</v>
       </c>
       <c r="E46">
         <v>95.28</v>
@@ -2730,10 +2730,10 @@
         <v>57</v>
       </c>
       <c r="C47">
-        <v>212</v>
+        <v>190</v>
       </c>
       <c r="D47">
-        <v>207.57</v>
+        <v>197.14</v>
       </c>
       <c r="E47">
         <v>95.44</v>
@@ -2747,10 +2747,10 @@
         <v>58</v>
       </c>
       <c r="C48">
-        <v>274</v>
+        <v>241</v>
       </c>
       <c r="D48">
-        <v>235</v>
+        <v>228.83</v>
       </c>
       <c r="E48">
         <v>95.59999999999999</v>
@@ -2764,10 +2764,10 @@
         <v>59</v>
       </c>
       <c r="C49">
-        <v>299</v>
+        <v>332</v>
       </c>
       <c r="D49">
-        <v>220.57</v>
+        <v>228.29</v>
       </c>
       <c r="E49">
         <v>95.76000000000001</v>
@@ -2781,10 +2781,10 @@
         <v>60</v>
       </c>
       <c r="C50">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="D50">
-        <v>132.38</v>
+        <v>132.5</v>
       </c>
       <c r="E50">
         <v>95.93000000000001</v>
@@ -2798,10 +2798,10 @@
         <v>61</v>
       </c>
       <c r="C51">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D51">
-        <v>107.75</v>
+        <v>105.5</v>
       </c>
       <c r="E51">
         <v>96.09</v>
@@ -2815,10 +2815,10 @@
         <v>62</v>
       </c>
       <c r="C52">
-        <v>268</v>
+        <v>284</v>
       </c>
       <c r="D52">
-        <v>262.62</v>
+        <v>269.62</v>
       </c>
       <c r="E52">
         <v>96.25</v>
@@ -2832,10 +2832,10 @@
         <v>63</v>
       </c>
       <c r="C53">
-        <v>257</v>
+        <v>227</v>
       </c>
       <c r="D53">
-        <v>228.12</v>
+        <v>228.62</v>
       </c>
       <c r="E53">
         <v>96.41</v>
@@ -2849,10 +2849,10 @@
         <v>64</v>
       </c>
       <c r="C54">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D54">
-        <v>207.12</v>
+        <v>197.75</v>
       </c>
       <c r="E54">
         <v>96.56999999999999</v>
@@ -2866,10 +2866,10 @@
         <v>65</v>
       </c>
       <c r="C55">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="D55">
-        <v>231.43</v>
+        <v>224.86</v>
       </c>
       <c r="E55">
         <v>96.73</v>
@@ -2883,10 +2883,10 @@
         <v>66</v>
       </c>
       <c r="C56">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D56">
-        <v>204.88</v>
+        <v>211.25</v>
       </c>
       <c r="E56">
         <v>96.89</v>
@@ -2900,10 +2900,10 @@
         <v>67</v>
       </c>
       <c r="C57">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D57">
-        <v>122.56</v>
+        <v>122.44</v>
       </c>
       <c r="E57">
         <v>97.06</v>
@@ -2917,10 +2917,10 @@
         <v>68</v>
       </c>
       <c r="C58">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D58">
-        <v>238.56</v>
+        <v>244.67</v>
       </c>
       <c r="E58">
         <v>97.38</v>
@@ -2937,7 +2937,7 @@
         <v>99</v>
       </c>
       <c r="D59">
-        <v>213.78</v>
+        <v>214.22</v>
       </c>
       <c r="E59">
         <v>97.54000000000001</v>
@@ -2951,10 +2951,10 @@
         <v>70</v>
       </c>
       <c r="C60">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D60">
-        <v>200.44</v>
+        <v>191.78</v>
       </c>
       <c r="E60">
         <v>97.7</v>
@@ -2968,10 +2968,10 @@
         <v>71</v>
       </c>
       <c r="C61">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="D61">
-        <v>221</v>
+        <v>214.12</v>
       </c>
       <c r="E61">
         <v>97.86</v>
@@ -2985,10 +2985,10 @@
         <v>72</v>
       </c>
       <c r="C62">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="D62">
-        <v>221.44</v>
+        <v>227.44</v>
       </c>
       <c r="E62">
         <v>98.03</v>
@@ -3002,10 +3002,10 @@
         <v>73</v>
       </c>
       <c r="C63">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="D63">
-        <v>115.9</v>
+        <v>116.5</v>
       </c>
       <c r="E63">
         <v>98.19</v>

</xml_diff>